<commit_message>
slides based on Geoff's talk
</commit_message>
<xml_diff>
--- a/_slides.xlsx
+++ b/_slides.xlsx
@@ -10,13 +10,14 @@
   <sheets>
     <sheet name="slides" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="values" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="old_slides" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>id</t>
   </si>
@@ -51,15 +52,120 @@
     <t>http://commons.wikimedia.org/wiki/File%3AIda_M_Tarbell_crop.jpg</t>
   </si>
   <si>
+    <t>in-this-together</t>
+  </si>
+  <si>
+    <t>slide-dark</t>
+  </si>
+  <si>
+    <t>in-this-together.jpg</t>
+  </si>
+  <si>
+    <t>my-kind-of-town</t>
+  </si>
+  <si>
+    <t>broken-fields</t>
+  </si>
+  <si>
+    <t>multiple-values</t>
+  </si>
+  <si>
+    <t>different-references</t>
+  </si>
+  <si>
+    <t>encoded-values</t>
+  </si>
+  <si>
+    <t>what-to-do</t>
+  </si>
+  <si>
+    <t>rule1</t>
+  </si>
+  <si>
+    <t>start-clean</t>
+  </si>
+  <si>
+    <t>toolkit</t>
+  </si>
+  <si>
+    <t>homework</t>
+  </si>
+  <si>
+    <t>inspection</t>
+  </si>
+  <si>
+    <t>quick-stats1</t>
+  </si>
+  <si>
+    <t>quick-stats2</t>
+  </si>
+  <si>
+    <t>refine_facet.png</t>
+  </si>
+  <si>
+    <t>quick-stats3</t>
+  </si>
+  <si>
+    <t>refine_cluster.png</t>
+  </si>
+  <si>
+    <t>decompose</t>
+  </si>
+  <si>
+    <t>do-i-have-to</t>
+  </si>
+  <si>
+    <t>do-i-have-to.jpg</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>_notes</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>This is my headline</t>
+  </si>
+  <si>
+    <t>Show key-&gt;value mapping -- print in template with {{ headline }}</t>
+  </si>
+  <si>
+    <t>google_analytics_id</t>
+  </si>
+  <si>
+    <t>Identifier for Google analytics</t>
+  </si>
+  <si>
+    <t>opengraph_image</t>
+  </si>
+  <si>
+    <t>OpenGraph image (Facebook, Pinterest, Google Plus), use full url</t>
+  </si>
+  <si>
+    <t>opengraph_description</t>
+  </si>
+  <si>
+    <t>OpenGraph description (Facebook, Pinterest, Google Plus)</t>
+  </si>
+  <si>
+    <t>twitter_description</t>
+  </si>
+  <si>
+    <t>Text for twitter</t>
+  </si>
+  <si>
     <t>case-study</t>
   </si>
   <si>
     <t>screenshot</t>
   </si>
   <si>
-    <t>rule1</t>
-  </si>
-  <si>
     <t>whats-a-workflow</t>
   </si>
   <si>
@@ -94,48 +200,6 @@
   </si>
   <si>
     <t>impact</t>
-  </si>
-  <si>
-    <t>key</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>_notes</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>This is my headline</t>
-  </si>
-  <si>
-    <t>Show key-&gt;value mapping -- print in template with {{ headline }}</t>
-  </si>
-  <si>
-    <t>google_analytics_id</t>
-  </si>
-  <si>
-    <t>Identifier for Google analytics</t>
-  </si>
-  <si>
-    <t>opengraph_image</t>
-  </si>
-  <si>
-    <t>OpenGraph image (Facebook, Pinterest, Google Plus), use full url</t>
-  </si>
-  <si>
-    <t>opengraph_description</t>
-  </si>
-  <si>
-    <t>OpenGraph description (Facebook, Pinterest, Google Plus)</t>
-  </si>
-  <si>
-    <t>twitter_description</t>
-  </si>
-  <si>
-    <t>Text for twitter</t>
   </si>
 </sst>
 </file>
@@ -351,14 +415,14 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -414,75 +478,100 @@
       <c r="A3" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="B3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -520,13 +609,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -534,13 +623,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -548,11 +637,11 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -560,11 +649,11 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -572,11 +661,11 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="6" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -584,11 +673,11 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="6" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -603,4 +692,106 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>